<commit_message>
updated project plan files
</commit_message>
<xml_diff>
--- a/docs/missing_semicolon_fall19.xlsx
+++ b/docs/missing_semicolon_fall19.xlsx
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -430,7 +430,7 @@
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>86.75 days?</t>
+          <t>68 days?</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
@@ -440,7 +440,7 @@
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>January 9, 2020 3:00 PM</t>
+          <t>December 13, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
@@ -1194,27 +1194,27 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>Dev testing</t>
+          <t>Sprint 1 complete</t>
         </is>
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>5 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>October 8, 2019 1:00 PM</t>
+          <t>October 14, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="G19" s="0" t="inlineStr">
         <is>
-          <t>October 15, 2019 12:00 PM</t>
+          <t>October 14, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H19" s="0" t="inlineStr">
         <is>
-          <t>16FS-75%</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I19" s="0" t="inlineStr">
@@ -1236,37 +1236,32 @@
       </c>
       <c r="C20" s="0" t="inlineStr">
         <is>
-          <t>Auto Scheduled</t>
+          <t>Manually Scheduled</t>
         </is>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>Sprint 1 complete</t>
+          <t>Sprint 2 Development</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>0 days</t>
+          <t>15 days?</t>
         </is>
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>October 15, 2019 12:00 PM</t>
+          <t>October 16, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G20" s="0" t="inlineStr">
         <is>
-          <t>October 15, 2019 12:00 PM</t>
-        </is>
-      </c>
-      <c r="H20" s="0" t="inlineStr">
-        <is>
-          <t>17</t>
+          <t>November 5, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I20" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1283,17 +1278,17 @@
       </c>
       <c r="C21" s="0" t="inlineStr">
         <is>
-          <t>Manually Scheduled</t>
+          <t>Auto Scheduled</t>
         </is>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>Sprint 2 Development</t>
+          <t>Development</t>
         </is>
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>14 days</t>
         </is>
       </c>
       <c r="F21" s="0" t="inlineStr">
@@ -1303,12 +1298,17 @@
       </c>
       <c r="G21" s="0" t="inlineStr">
         <is>
-          <t>November 5, 2019 5:00 PM</t>
+          <t>November 4, 2019 5:00 PM</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t>17</t>
         </is>
       </c>
       <c r="I21" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1330,27 +1330,27 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>Sprint 3 planning</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>14 days</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
-          <t>October 16, 2019 8:00 AM</t>
+          <t>November 5, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G22" s="0" t="inlineStr">
         <is>
-          <t>November 4, 2019 5:00 PM</t>
+          <t>November 5, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H22" s="0" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I22" s="0" t="inlineStr">
@@ -1377,27 +1377,27 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>Dev testing</t>
+          <t>Sprint 2 complete</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>11 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t>October 21, 2019 1:00 PM</t>
+          <t>November 5, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="G23" s="0" t="inlineStr">
         <is>
-          <t>November 5, 2019 12:00 PM</t>
+          <t>November 5, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H23" s="0" t="inlineStr">
         <is>
-          <t>20FS-75%</t>
+          <t>20</t>
         </is>
       </c>
       <c r="I23" s="0" t="inlineStr">
@@ -1419,37 +1419,32 @@
       </c>
       <c r="C24" s="0" t="inlineStr">
         <is>
-          <t>Auto Scheduled</t>
+          <t>Manually Scheduled</t>
         </is>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>Sprint 2 complete</t>
+          <t>Sprint 3 development</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>0 days</t>
+          <t>20 days?</t>
         </is>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>November 5, 2019 12:00 PM</t>
+          <t>November 6, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G24" s="0" t="inlineStr">
         <is>
-          <t>November 5, 2019 12:00 PM</t>
-        </is>
-      </c>
-      <c r="H24" s="0" t="inlineStr">
-        <is>
-          <t>21</t>
+          <t>December 3, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I24" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1466,17 +1461,17 @@
       </c>
       <c r="C25" s="0" t="inlineStr">
         <is>
-          <t>Manually Scheduled</t>
+          <t>Auto Scheduled</t>
         </is>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>Sprint 3 development</t>
+          <t>Development</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
-          <t>20 days?</t>
+          <t>16 days</t>
         </is>
       </c>
       <c r="F25" s="0" t="inlineStr">
@@ -1486,12 +1481,17 @@
       </c>
       <c r="G25" s="0" t="inlineStr">
         <is>
-          <t>December 3, 2019 5:00 PM</t>
+          <t>November 27, 2019 5:00 PM</t>
+        </is>
+      </c>
+      <c r="H25" s="0" t="inlineStr">
+        <is>
+          <t>21</t>
         </is>
       </c>
       <c r="I25" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1513,27 +1513,27 @@
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>Development complete</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
         <is>
-          <t>19 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>November 6, 2019 8:00 AM</t>
+          <t>December 2, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G26" s="0" t="inlineStr">
         <is>
-          <t>December 2, 2019 5:00 PM</t>
+          <t>December 2, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="H26" s="0" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I26" s="0" t="inlineStr">
@@ -1555,37 +1555,32 @@
       </c>
       <c r="C27" s="0" t="inlineStr">
         <is>
-          <t>Manually Scheduled</t>
+          <t>Auto Scheduled</t>
         </is>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>Dev testing</t>
+          <t>Testing</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>48 days</t>
         </is>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>November 12, 2019 3:00 PM</t>
+          <t>October 2, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G27" s="0" t="inlineStr">
         <is>
-          <t>December 3, 2019 3:00 PM</t>
-        </is>
-      </c>
-      <c r="H27" s="0" t="inlineStr">
-        <is>
-          <t>24FS-75%</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I27" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1607,27 +1602,27 @@
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>Development complete</t>
+          <t>Develop unit test plans using product specifications</t>
         </is>
       </c>
       <c r="E28" s="0" t="inlineStr">
         <is>
-          <t>0 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
-          <t>December 3, 2019 3:00 PM</t>
+          <t>October 2, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G28" s="0" t="inlineStr">
         <is>
-          <t>December 3, 2019 3:00 PM</t>
+          <t>October 7, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H28" s="0" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>12</t>
         </is>
       </c>
       <c r="I28" s="0" t="inlineStr">
@@ -1649,32 +1644,32 @@
       </c>
       <c r="C29" s="0" t="inlineStr">
         <is>
-          <t>Auto Scheduled</t>
+          <t>Manually Scheduled</t>
         </is>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>Testing</t>
+          <t>Unit Testing</t>
         </is>
       </c>
       <c r="E29" s="0" t="inlineStr">
         <is>
-          <t>71.75 days</t>
+          <t>36 days</t>
         </is>
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
-          <t>October 2, 2019 8:00 AM</t>
+          <t>October 16, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G29" s="0" t="inlineStr">
         <is>
-          <t>January 9, 2020 3:00 PM</t>
+          <t>December 4, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I29" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1691,7 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>Develop unit test plans using product specifications</t>
+          <t>Sprint 1 testing</t>
         </is>
       </c>
       <c r="E30" s="0" t="inlineStr">
@@ -1706,22 +1701,22 @@
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
-          <t>October 2, 2019 8:00 AM</t>
+          <t>October 15, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G30" s="0" t="inlineStr">
         <is>
-          <t>October 7, 2019 5:00 PM</t>
+          <t>October 18, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H30" s="0" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I30" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1743,27 +1738,32 @@
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>Unit Testing</t>
+          <t>Sprint 2 testing</t>
         </is>
       </c>
       <c r="E31" s="0" t="inlineStr">
         <is>
-          <t>15 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="F31" s="0" t="inlineStr">
         <is>
-          <t>December 3, 2019 3:00 PM</t>
+          <t>November 5, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G31" s="0" t="inlineStr">
         <is>
-          <t>December 24, 2019 3:00 PM</t>
+          <t>November 8, 2019 5:00 PM</t>
+        </is>
+      </c>
+      <c r="H31" s="0" t="inlineStr">
+        <is>
+          <t>19</t>
         </is>
       </c>
       <c r="I31" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1785,27 +1785,27 @@
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t>Review modular code</t>
+          <t>Sprint 3 testing</t>
         </is>
       </c>
       <c r="E32" s="0" t="inlineStr">
         <is>
-          <t>5 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
-          <t>December 3, 2019 3:00 PM</t>
+          <t>December 2, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G32" s="0" t="inlineStr">
         <is>
-          <t>December 10, 2019 3:00 PM</t>
+          <t>December 4, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H32" s="0" t="inlineStr">
         <is>
-          <t>28,26</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I32" s="0" t="inlineStr">
@@ -1832,27 +1832,27 @@
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t>Test component modules to product specifications</t>
+          <t>Unit testing complete</t>
         </is>
       </c>
       <c r="E33" s="0" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
-          <t>December 10, 2019 3:00 PM</t>
+          <t>December 4, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="G33" s="0" t="inlineStr">
         <is>
-          <t>December 12, 2019 3:00 PM</t>
+          <t>December 4, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H33" s="0" t="inlineStr">
         <is>
-          <t>26,30</t>
+          <t>30</t>
         </is>
       </c>
       <c r="I33" s="0" t="inlineStr">
@@ -1879,32 +1879,27 @@
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
-          <t>Identify anomalies to product specifications</t>
+          <t>Integration Testing</t>
         </is>
       </c>
       <c r="E34" s="0" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="F34" s="0" t="inlineStr">
         <is>
-          <t>December 12, 2019 3:00 PM</t>
+          <t>December 5, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G34" s="0" t="inlineStr">
         <is>
-          <t>December 17, 2019 3:00 PM</t>
-        </is>
-      </c>
-      <c r="H34" s="0" t="inlineStr">
-        <is>
-          <t>31</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I34" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1926,27 +1921,27 @@
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
-          <t>Modify code</t>
+          <t>Test module integration</t>
         </is>
       </c>
       <c r="E35" s="0" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
-          <t>December 17, 2019 3:00 PM</t>
+          <t>December 5, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G35" s="0" t="inlineStr">
         <is>
-          <t>December 20, 2019 3:00 PM</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H35" s="0" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>31</t>
         </is>
       </c>
       <c r="I35" s="0" t="inlineStr">
@@ -1973,22 +1968,22 @@
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
-          <t>Re-test modified code</t>
+          <t>Integration testing complete</t>
         </is>
       </c>
       <c r="E36" s="0" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F36" s="0" t="inlineStr">
         <is>
-          <t>December 20, 2019 3:00 PM</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="G36" s="0" t="inlineStr">
         <is>
-          <t>December 24, 2019 3:00 PM</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H36" s="0" t="inlineStr">
@@ -2020,32 +2015,27 @@
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
-          <t>Unit testing complete</t>
+          <t>Documentation</t>
         </is>
       </c>
       <c r="E37" s="0" t="inlineStr">
         <is>
-          <t>0 days</t>
+          <t>39 days</t>
         </is>
       </c>
       <c r="F37" s="0" t="inlineStr">
         <is>
-          <t>December 24, 2019 3:00 PM</t>
+          <t>October 15, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G37" s="0" t="inlineStr">
         <is>
-          <t>December 24, 2019 3:00 PM</t>
-        </is>
-      </c>
-      <c r="H37" s="0" t="inlineStr">
-        <is>
-          <t>34</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I37" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2062,27 +2052,32 @@
       </c>
       <c r="C38" s="0" t="inlineStr">
         <is>
-          <t>Auto Scheduled</t>
+          <t>Manually Scheduled</t>
         </is>
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
-          <t>Integration Testing</t>
+          <t>Write Sprint 1 documentation</t>
         </is>
       </c>
       <c r="E38" s="0" t="inlineStr">
         <is>
-          <t>12 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="F38" s="0" t="inlineStr">
         <is>
-          <t>December 24, 2019 3:00 PM</t>
+          <t>October 15, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G38" s="0" t="inlineStr">
         <is>
-          <t>January 9, 2020 3:00 PM</t>
+          <t>October 17, 2019 5:00 PM</t>
+        </is>
+      </c>
+      <c r="H38" s="0" t="inlineStr">
+        <is>
+          <t>17</t>
         </is>
       </c>
       <c r="I38" s="0" t="inlineStr">
@@ -2109,32 +2104,32 @@
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
-          <t>Test module integration</t>
+          <t>Write Sprint 2 documentation</t>
         </is>
       </c>
       <c r="E39" s="0" t="inlineStr">
         <is>
-          <t>5 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="F39" s="0" t="inlineStr">
         <is>
-          <t>December 24, 2019 3:00 PM</t>
+          <t>November 5, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G39" s="0" t="inlineStr">
         <is>
-          <t>December 31, 2019 3:00 PM</t>
+          <t>November 7, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H39" s="0" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>19</t>
         </is>
       </c>
       <c r="I39" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2156,32 +2151,27 @@
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
-          <t>Identify anomalies to specifications</t>
+          <t>Write Sprint 3 documentation</t>
         </is>
       </c>
       <c r="E40" s="0" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>3 days</t>
         </is>
       </c>
       <c r="F40" s="0" t="inlineStr">
         <is>
-          <t>December 31, 2019 3:00 PM</t>
+          <t>December 2, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G40" s="0" t="inlineStr">
         <is>
-          <t>January 2, 2020 3:00 PM</t>
-        </is>
-      </c>
-      <c r="H40" s="0" t="inlineStr">
-        <is>
-          <t>37</t>
+          <t>December 4, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I40" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2203,22 +2193,22 @@
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
-          <t>Modify code</t>
+          <t>Review and Format API documentation</t>
         </is>
       </c>
       <c r="E41" s="0" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>2 days</t>
         </is>
       </c>
       <c r="F41" s="0" t="inlineStr">
         <is>
-          <t>January 2, 2020 3:00 PM</t>
+          <t>December 5, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G41" s="0" t="inlineStr">
         <is>
-          <t>January 7, 2020 3:00 PM</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H41" s="0" t="inlineStr">
@@ -2228,7 +2218,7 @@
       </c>
       <c r="I41" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2250,22 +2240,22 @@
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
-          <t>Re-test modified code</t>
+          <t>Documentation complete</t>
         </is>
       </c>
       <c r="E42" s="0" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F42" s="0" t="inlineStr">
         <is>
-          <t>January 7, 2020 3:00 PM</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="G42" s="0" t="inlineStr">
         <is>
-          <t>January 9, 2020 3:00 PM</t>
+          <t>December 6, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H42" s="0" t="inlineStr">
@@ -2275,7 +2265,7 @@
       </c>
       <c r="I42" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2297,32 +2287,27 @@
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
-          <t>Integration testing complete</t>
+          <t>Deployment</t>
         </is>
       </c>
       <c r="E43" s="0" t="inlineStr">
         <is>
-          <t>0 days</t>
+          <t>49 days</t>
         </is>
       </c>
       <c r="F43" s="0" t="inlineStr">
         <is>
-          <t>January 9, 2020 3:00 PM</t>
+          <t>October 2, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G43" s="0" t="inlineStr">
         <is>
-          <t>January 9, 2020 3:00 PM</t>
-        </is>
-      </c>
-      <c r="H43" s="0" t="inlineStr">
-        <is>
-          <t>40</t>
+          <t>December 9, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I43" s="0" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2344,27 +2329,32 @@
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
-          <t>Documentation</t>
+          <t>Determine final deployment strategy</t>
         </is>
       </c>
       <c r="E44" s="0" t="inlineStr">
         <is>
-          <t>41 days</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="F44" s="0" t="inlineStr">
         <is>
-          <t>September 11, 2019 8:00 AM</t>
+          <t>October 2, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G44" s="0" t="inlineStr">
         <is>
-          <t>November 6, 2019 5:00 PM</t>
+          <t>October 2, 2019 5:00 PM</t>
+        </is>
+      </c>
+      <c r="H44" s="0" t="inlineStr">
+        <is>
+          <t>12</t>
         </is>
       </c>
       <c r="I44" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -2386,7 +2376,7 @@
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
-          <t>Develop Help specification</t>
+          <t>Develop deployment methodology</t>
         </is>
       </c>
       <c r="E45" s="0" t="inlineStr">
@@ -2396,12 +2386,17 @@
       </c>
       <c r="F45" s="0" t="inlineStr">
         <is>
-          <t>September 11, 2019 8:00 AM</t>
+          <t>October 3, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G45" s="0" t="inlineStr">
         <is>
-          <t>September 11, 2019 5:00 PM</t>
+          <t>October 3, 2019 5:00 PM</t>
+        </is>
+      </c>
+      <c r="H45" s="0" t="inlineStr">
+        <is>
+          <t>42</t>
         </is>
       </c>
       <c r="I45" s="0" t="inlineStr">
@@ -2428,27 +2423,27 @@
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
-          <t>Develop Help system</t>
+          <t>Secure deployment resources</t>
         </is>
       </c>
       <c r="E46" s="0" t="inlineStr">
         <is>
-          <t>3 wks</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="F46" s="0" t="inlineStr">
         <is>
-          <t>October 10, 2019 8:00 AM</t>
+          <t>October 4, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G46" s="0" t="inlineStr">
         <is>
-          <t>October 30, 2019 5:00 PM</t>
+          <t>October 4, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H46" s="0" t="inlineStr">
         <is>
-          <t>43,16FS-50%</t>
+          <t>43</t>
         </is>
       </c>
       <c r="I46" s="0" t="inlineStr">
@@ -2475,27 +2470,27 @@
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
-          <t>Review Help documentation</t>
+          <t>Deploy software</t>
         </is>
       </c>
       <c r="E47" s="0" t="inlineStr">
         <is>
-          <t>3 days</t>
+          <t>1 day</t>
         </is>
       </c>
       <c r="F47" s="0" t="inlineStr">
         <is>
-          <t>October 31, 2019 8:00 AM</t>
+          <t>December 9, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G47" s="0" t="inlineStr">
         <is>
-          <t>November 4, 2019 5:00 PM</t>
+          <t>December 9, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H47" s="0" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>34</t>
         </is>
       </c>
       <c r="I47" s="0" t="inlineStr">
@@ -2522,22 +2517,22 @@
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
-          <t>Incorporate Help documentation feedback</t>
+          <t>Deployment complete</t>
         </is>
       </c>
       <c r="E48" s="0" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F48" s="0" t="inlineStr">
         <is>
-          <t>November 5, 2019 8:00 AM</t>
+          <t>December 9, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="G48" s="0" t="inlineStr">
         <is>
-          <t>November 6, 2019 5:00 PM</t>
+          <t>December 9, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H48" s="0" t="inlineStr">
@@ -2569,27 +2564,27 @@
       </c>
       <c r="D49" s="0" t="inlineStr">
         <is>
-          <t>Develop user manuals specifications</t>
+          <t>Post Implementation Review</t>
         </is>
       </c>
       <c r="E49" s="0" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="F49" s="0" t="inlineStr">
         <is>
-          <t>September 11, 2019 8:00 AM</t>
+          <t>December 10, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G49" s="0" t="inlineStr">
         <is>
-          <t>September 12, 2019 5:00 PM</t>
+          <t>December 13, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="I49" s="0" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -2611,27 +2606,27 @@
       </c>
       <c r="D50" s="0" t="inlineStr">
         <is>
-          <t>Develop user manuals</t>
+          <t>Wait for final grade!</t>
         </is>
       </c>
       <c r="E50" s="0" t="inlineStr">
         <is>
-          <t>3 wks</t>
+          <t>4 days</t>
         </is>
       </c>
       <c r="F50" s="0" t="inlineStr">
         <is>
-          <t>October 10, 2019 8:00 AM</t>
+          <t>December 10, 2019 8:00 AM</t>
         </is>
       </c>
       <c r="G50" s="0" t="inlineStr">
         <is>
-          <t>October 30, 2019 5:00 PM</t>
+          <t>December 13, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H50" s="0" t="inlineStr">
         <is>
-          <t>47,16FS-50%</t>
+          <t>46</t>
         </is>
       </c>
       <c r="I50" s="0" t="inlineStr">
@@ -2658,22 +2653,22 @@
       </c>
       <c r="D51" s="0" t="inlineStr">
         <is>
-          <t>Review all user documentation</t>
+          <t>Post implementation review complete</t>
         </is>
       </c>
       <c r="E51" s="0" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F51" s="0" t="inlineStr">
         <is>
-          <t>October 31, 2019 8:00 AM</t>
+          <t>December 13, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="G51" s="0" t="inlineStr">
         <is>
-          <t>November 1, 2019 5:00 PM</t>
+          <t>December 13, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H51" s="0" t="inlineStr">
@@ -2705,22 +2700,22 @@
       </c>
       <c r="D52" s="0" t="inlineStr">
         <is>
-          <t>Incorporate user documentation feedback</t>
+          <t>Software development template complete</t>
         </is>
       </c>
       <c r="E52" s="0" t="inlineStr">
         <is>
-          <t>2 days</t>
+          <t>0 days</t>
         </is>
       </c>
       <c r="F52" s="0" t="inlineStr">
         <is>
-          <t>November 4, 2019 8:00 AM</t>
+          <t>December 13, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="G52" s="0" t="inlineStr">
         <is>
-          <t>November 5, 2019 5:00 PM</t>
+          <t>December 13, 2019 5:00 PM</t>
         </is>
       </c>
       <c r="H52" s="0" t="inlineStr">
@@ -2729,649 +2724,6 @@
         </is>
       </c>
       <c r="I52" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="53">
-      <c r="A53" s="0" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
-      </c>
-      <c r="B53" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C53" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D53" s="0" t="inlineStr">
-        <is>
-          <t>Documentation complete</t>
-        </is>
-      </c>
-      <c r="E53" s="0" t="inlineStr">
-        <is>
-          <t>0 days</t>
-        </is>
-      </c>
-      <c r="F53" s="0" t="inlineStr">
-        <is>
-          <t>November 6, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="G53" s="0" t="inlineStr">
-        <is>
-          <t>November 6, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H53" s="0" t="inlineStr">
-        <is>
-          <t>50,46</t>
-        </is>
-      </c>
-      <c r="I53" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="54">
-      <c r="A54" s="0" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
-      </c>
-      <c r="B54" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C54" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D54" s="0" t="inlineStr">
-        <is>
-          <t>Deployment</t>
-        </is>
-      </c>
-      <c r="E54" s="0" t="inlineStr">
-        <is>
-          <t>5 days</t>
-        </is>
-      </c>
-      <c r="F54" s="0" t="inlineStr">
-        <is>
-          <t>September 11, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G54" s="0" t="inlineStr">
-        <is>
-          <t>September 17, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="I54" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="55">
-      <c r="A55" s="0" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="B55" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C55" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D55" s="0" t="inlineStr">
-        <is>
-          <t>Determine final deployment strategy</t>
-        </is>
-      </c>
-      <c r="E55" s="0" t="inlineStr">
-        <is>
-          <t>1 day</t>
-        </is>
-      </c>
-      <c r="F55" s="0" t="inlineStr">
-        <is>
-          <t>September 11, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G55" s="0" t="inlineStr">
-        <is>
-          <t>September 11, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="I55" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="56">
-      <c r="A56" s="0" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="B56" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C56" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D56" s="0" t="inlineStr">
-        <is>
-          <t>Develop deployment methodology</t>
-        </is>
-      </c>
-      <c r="E56" s="0" t="inlineStr">
-        <is>
-          <t>1 day</t>
-        </is>
-      </c>
-      <c r="F56" s="0" t="inlineStr">
-        <is>
-          <t>September 12, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G56" s="0" t="inlineStr">
-        <is>
-          <t>September 12, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H56" s="0" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
-      </c>
-      <c r="I56" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="57">
-      <c r="A57" s="0" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="B57" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C57" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D57" s="0" t="inlineStr">
-        <is>
-          <t>Secure deployment resources</t>
-        </is>
-      </c>
-      <c r="E57" s="0" t="inlineStr">
-        <is>
-          <t>1 day</t>
-        </is>
-      </c>
-      <c r="F57" s="0" t="inlineStr">
-        <is>
-          <t>September 13, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G57" s="0" t="inlineStr">
-        <is>
-          <t>September 13, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H57" s="0" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="I57" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="58">
-      <c r="A58" s="0" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
-      </c>
-      <c r="B58" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C58" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D58" s="0" t="inlineStr">
-        <is>
-          <t>Train support staff</t>
-        </is>
-      </c>
-      <c r="E58" s="0" t="inlineStr">
-        <is>
-          <t>1 day</t>
-        </is>
-      </c>
-      <c r="F58" s="0" t="inlineStr">
-        <is>
-          <t>September 16, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G58" s="0" t="inlineStr">
-        <is>
-          <t>September 16, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H58" s="0" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="I58" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="59">
-      <c r="A59" s="0" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
-      </c>
-      <c r="B59" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C59" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D59" s="0" t="inlineStr">
-        <is>
-          <t>Deploy software</t>
-        </is>
-      </c>
-      <c r="E59" s="0" t="inlineStr">
-        <is>
-          <t>1 day</t>
-        </is>
-      </c>
-      <c r="F59" s="0" t="inlineStr">
-        <is>
-          <t>September 17, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G59" s="0" t="inlineStr">
-        <is>
-          <t>September 17, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H59" s="0" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
-      </c>
-      <c r="I59" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="60">
-      <c r="A60" s="0" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
-      </c>
-      <c r="B60" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C60" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D60" s="0" t="inlineStr">
-        <is>
-          <t>Deployment complete</t>
-        </is>
-      </c>
-      <c r="E60" s="0" t="inlineStr">
-        <is>
-          <t>0 days</t>
-        </is>
-      </c>
-      <c r="F60" s="0" t="inlineStr">
-        <is>
-          <t>September 17, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="G60" s="0" t="inlineStr">
-        <is>
-          <t>September 17, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H60" s="0" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
-      </c>
-      <c r="I60" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="61">
-      <c r="A61" s="0" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
-      </c>
-      <c r="B61" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C61" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D61" s="0" t="inlineStr">
-        <is>
-          <t>Post Implementation Review</t>
-        </is>
-      </c>
-      <c r="E61" s="0" t="inlineStr">
-        <is>
-          <t>3 days</t>
-        </is>
-      </c>
-      <c r="F61" s="0" t="inlineStr">
-        <is>
-          <t>September 18, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G61" s="0" t="inlineStr">
-        <is>
-          <t>September 20, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="I61" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="62">
-      <c r="A62" s="0" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="B62" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C62" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D62" s="0" t="inlineStr">
-        <is>
-          <t>Document lessons learned</t>
-        </is>
-      </c>
-      <c r="E62" s="0" t="inlineStr">
-        <is>
-          <t>1 day</t>
-        </is>
-      </c>
-      <c r="F62" s="0" t="inlineStr">
-        <is>
-          <t>September 18, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G62" s="0" t="inlineStr">
-        <is>
-          <t>September 18, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H62" s="0" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
-      </c>
-      <c r="I62" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="63">
-      <c r="A63" s="0" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="B63" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C63" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D63" s="0" t="inlineStr">
-        <is>
-          <t>Distribute to team members</t>
-        </is>
-      </c>
-      <c r="E63" s="0" t="inlineStr">
-        <is>
-          <t>1 day</t>
-        </is>
-      </c>
-      <c r="F63" s="0" t="inlineStr">
-        <is>
-          <t>September 19, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G63" s="0" t="inlineStr">
-        <is>
-          <t>September 19, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H63" s="0" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="I63" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="64">
-      <c r="A64" s="0" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="B64" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C64" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D64" s="0" t="inlineStr">
-        <is>
-          <t>Create software maintenance team</t>
-        </is>
-      </c>
-      <c r="E64" s="0" t="inlineStr">
-        <is>
-          <t>1 day</t>
-        </is>
-      </c>
-      <c r="F64" s="0" t="inlineStr">
-        <is>
-          <t>September 20, 2019 8:00 AM</t>
-        </is>
-      </c>
-      <c r="G64" s="0" t="inlineStr">
-        <is>
-          <t>September 20, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H64" s="0" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
-      </c>
-      <c r="I64" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="65">
-      <c r="A65" s="0" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
-      </c>
-      <c r="B65" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C65" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D65" s="0" t="inlineStr">
-        <is>
-          <t>Post implementation review complete</t>
-        </is>
-      </c>
-      <c r="E65" s="0" t="inlineStr">
-        <is>
-          <t>0 days</t>
-        </is>
-      </c>
-      <c r="F65" s="0" t="inlineStr">
-        <is>
-          <t>September 20, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="G65" s="0" t="inlineStr">
-        <is>
-          <t>September 20, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H65" s="0" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="I65" s="0" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="66">
-      <c r="A66" s="0" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
-      </c>
-      <c r="B66" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="C66" s="0" t="inlineStr">
-        <is>
-          <t>Auto Scheduled</t>
-        </is>
-      </c>
-      <c r="D66" s="0" t="inlineStr">
-        <is>
-          <t>Software development template complete</t>
-        </is>
-      </c>
-      <c r="E66" s="0" t="inlineStr">
-        <is>
-          <t>0 days</t>
-        </is>
-      </c>
-      <c r="F66" s="0" t="inlineStr">
-        <is>
-          <t>September 20, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="G66" s="0" t="inlineStr">
-        <is>
-          <t>September 20, 2019 5:00 PM</t>
-        </is>
-      </c>
-      <c r="H66" s="0" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
-      </c>
-      <c r="I66" s="0" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3526,12 +2878,12 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Brian (Proj Mgr)</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
@@ -3563,12 +2915,12 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Lindsay (Analyst)</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>L</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
@@ -3600,12 +2952,12 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>Hailey (Dev)</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>H</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
@@ -3637,12 +2989,12 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>QA Team</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
@@ -3711,7 +3063,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Technical Communicators</t>
+          <t>Tech Writers</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
@@ -3784,7 +3136,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -3881,7 +3233,7 @@
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Brian (Proj Mgr)</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
@@ -3908,7 +3260,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Lindsay (Analyst)</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
@@ -3935,7 +3287,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>Hailey (Dev)</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
@@ -3962,7 +3314,7 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Brian (Proj Mgr)</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
@@ -3989,7 +3341,7 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Lindsay (Analyst)</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
@@ -4016,7 +3368,7 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Brian (Proj Mgr)</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
@@ -4043,7 +3395,7 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Lindsay (Analyst)</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
@@ -4070,7 +3422,7 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Analyst</t>
+          <t>Lindsay (Analyst)</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
@@ -4097,12 +3449,12 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>Project Manager</t>
+          <t>Brian (Proj Mgr)</t>
         </is>
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D12" s="0" t="inlineStr">
@@ -4124,7 +3476,7 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>Hailey (Dev)</t>
         </is>
       </c>
       <c r="C13" s="0" t="inlineStr">
@@ -4151,7 +3503,7 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>Hailey (Dev)</t>
         </is>
       </c>
       <c r="C14" s="0" t="inlineStr">
@@ -4178,7 +3530,7 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>Hailey (Dev)</t>
         </is>
       </c>
       <c r="C15" s="0" t="inlineStr">
@@ -4200,12 +3552,12 @@
     <row outlineLevel="0" r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>Dev testing</t>
+          <t>Development</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>Hailey (Dev)</t>
         </is>
       </c>
       <c r="C16" s="0" t="inlineStr">
@@ -4215,12 +3567,12 @@
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>33.33h</t>
+          <t>112h</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>83%</t>
+          <t>100%</t>
         </is>
       </c>
     </row>
@@ -4232,7 +3584,7 @@
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>Hailey (Dev)</t>
         </is>
       </c>
       <c r="C17" s="0" t="inlineStr">
@@ -4242,7 +3594,7 @@
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>112h</t>
+          <t>128h</t>
         </is>
       </c>
       <c r="E17" s="0" t="inlineStr">
@@ -4254,12 +3606,12 @@
     <row outlineLevel="0" r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>Dev testing</t>
+          <t>Develop unit test plans using product specifications</t>
         </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>QA Team</t>
         </is>
       </c>
       <c r="C18" s="0" t="inlineStr">
@@ -4269,7 +3621,7 @@
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>88h</t>
+          <t>32h</t>
         </is>
       </c>
       <c r="E18" s="0" t="inlineStr">
@@ -4281,12 +3633,12 @@
     <row outlineLevel="0" r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>Development</t>
+          <t>Sprint 1 testing</t>
         </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>QA Team</t>
         </is>
       </c>
       <c r="C19" s="0" t="inlineStr">
@@ -4296,7 +3648,7 @@
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>152h</t>
+          <t>32h</t>
         </is>
       </c>
       <c r="E19" s="0" t="inlineStr">
@@ -4308,12 +3660,12 @@
     <row outlineLevel="0" r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>Dev testing</t>
+          <t>Sprint 2 testing</t>
         </is>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>Developer</t>
+          <t>QA Team</t>
         </is>
       </c>
       <c r="C20" s="0" t="inlineStr">
@@ -4323,7 +3675,7 @@
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>120h</t>
+          <t>32h</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
@@ -4335,12 +3687,12 @@
     <row outlineLevel="0" r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>Develop unit test plans using product specifications</t>
+          <t>Sprint 3 testing</t>
         </is>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>QA Team</t>
         </is>
       </c>
       <c r="C21" s="0" t="inlineStr">
@@ -4350,7 +3702,7 @@
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>32h</t>
+          <t>24h</t>
         </is>
       </c>
       <c r="E21" s="0" t="inlineStr">
@@ -4362,12 +3714,12 @@
     <row outlineLevel="0" r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>Review modular code</t>
+          <t>Test module integration</t>
         </is>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>QA Team</t>
         </is>
       </c>
       <c r="C22" s="0" t="inlineStr">
@@ -4377,7 +3729,7 @@
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>40h</t>
+          <t>16h</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
@@ -4389,12 +3741,12 @@
     <row outlineLevel="0" r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>Test component modules to product specifications</t>
+          <t>Write Sprint 1 documentation</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>Tech Writers</t>
         </is>
       </c>
       <c r="C23" s="0" t="inlineStr">
@@ -4404,7 +3756,7 @@
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>16h</t>
+          <t>24h</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
@@ -4416,12 +3768,12 @@
     <row outlineLevel="0" r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>Identify anomalies to product specifications</t>
+          <t>Write Sprint 2 documentation</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>Tech Writers</t>
         </is>
       </c>
       <c r="C24" s="0" t="inlineStr">
@@ -4443,12 +3795,12 @@
     <row outlineLevel="0" r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>Modify code</t>
+          <t>Review and Format API documentation</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>Tech Writers</t>
         </is>
       </c>
       <c r="C25" s="0" t="inlineStr">
@@ -4458,7 +3810,7 @@
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>24h</t>
+          <t>16h</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
@@ -4470,22 +3822,22 @@
     <row outlineLevel="0" r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>Re-test modified code</t>
+          <t>Determine final deployment strategy</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>Deployment Team</t>
         </is>
       </c>
       <c r="C26" s="0" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>16h</t>
+          <t>8h</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
@@ -4497,22 +3849,22 @@
     <row outlineLevel="0" r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>Test module integration</t>
+          <t>Develop deployment methodology</t>
         </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>Deployment Team</t>
         </is>
       </c>
       <c r="C27" s="0" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>40h</t>
+          <t>8h</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
@@ -4524,22 +3876,22 @@
     <row outlineLevel="0" r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>Identify anomalies to specifications</t>
+          <t>Secure deployment resources</t>
         </is>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>Deployment Team</t>
         </is>
       </c>
       <c r="C28" s="0" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>16h</t>
+          <t>8h</t>
         </is>
       </c>
       <c r="E28" s="0" t="inlineStr">
@@ -4551,12 +3903,12 @@
     <row outlineLevel="0" r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>Modify code</t>
+          <t>Deploy software</t>
         </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>Deployment Team</t>
         </is>
       </c>
       <c r="C29" s="0" t="inlineStr">
@@ -4566,7 +3918,7 @@
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>24h</t>
+          <t>8h</t>
         </is>
       </c>
       <c r="E29" s="0" t="inlineStr">
@@ -4578,12 +3930,12 @@
     <row outlineLevel="0" r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>Re-test modified code</t>
+          <t>Wait for final grade!</t>
         </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>Testers</t>
+          <t>Brian (Proj Mgr)</t>
         </is>
       </c>
       <c r="C30" s="0" t="inlineStr">
@@ -4593,442 +3945,10 @@
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>16h</t>
+          <t>32h</t>
         </is>
       </c>
       <c r="E30" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="31">
-      <c r="A31" s="0" t="inlineStr">
-        <is>
-          <t>Develop Help specification</t>
-        </is>
-      </c>
-      <c r="B31" s="0" t="inlineStr">
-        <is>
-          <t>Technical Communicators</t>
-        </is>
-      </c>
-      <c r="C31" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D31" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E31" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="32">
-      <c r="A32" s="0" t="inlineStr">
-        <is>
-          <t>Develop Help system</t>
-        </is>
-      </c>
-      <c r="B32" s="0" t="inlineStr">
-        <is>
-          <t>Technical Communicators</t>
-        </is>
-      </c>
-      <c r="C32" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D32" s="0" t="inlineStr">
-        <is>
-          <t>120h</t>
-        </is>
-      </c>
-      <c r="E32" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="33">
-      <c r="A33" s="0" t="inlineStr">
-        <is>
-          <t>Review Help documentation</t>
-        </is>
-      </c>
-      <c r="B33" s="0" t="inlineStr">
-        <is>
-          <t>Technical Communicators</t>
-        </is>
-      </c>
-      <c r="C33" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D33" s="0" t="inlineStr">
-        <is>
-          <t>24h</t>
-        </is>
-      </c>
-      <c r="E33" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="34">
-      <c r="A34" s="0" t="inlineStr">
-        <is>
-          <t>Incorporate Help documentation feedback</t>
-        </is>
-      </c>
-      <c r="B34" s="0" t="inlineStr">
-        <is>
-          <t>Technical Communicators</t>
-        </is>
-      </c>
-      <c r="C34" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D34" s="0" t="inlineStr">
-        <is>
-          <t>16h</t>
-        </is>
-      </c>
-      <c r="E34" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="35">
-      <c r="A35" s="0" t="inlineStr">
-        <is>
-          <t>Develop user manuals specifications</t>
-        </is>
-      </c>
-      <c r="B35" s="0" t="inlineStr">
-        <is>
-          <t>Technical Communicators</t>
-        </is>
-      </c>
-      <c r="C35" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D35" s="0" t="inlineStr">
-        <is>
-          <t>16h</t>
-        </is>
-      </c>
-      <c r="E35" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="36">
-      <c r="A36" s="0" t="inlineStr">
-        <is>
-          <t>Develop user manuals</t>
-        </is>
-      </c>
-      <c r="B36" s="0" t="inlineStr">
-        <is>
-          <t>Technical Communicators</t>
-        </is>
-      </c>
-      <c r="C36" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D36" s="0" t="inlineStr">
-        <is>
-          <t>120h</t>
-        </is>
-      </c>
-      <c r="E36" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="37">
-      <c r="A37" s="0" t="inlineStr">
-        <is>
-          <t>Review all user documentation</t>
-        </is>
-      </c>
-      <c r="B37" s="0" t="inlineStr">
-        <is>
-          <t>Technical Communicators</t>
-        </is>
-      </c>
-      <c r="C37" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D37" s="0" t="inlineStr">
-        <is>
-          <t>16h</t>
-        </is>
-      </c>
-      <c r="E37" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="38">
-      <c r="A38" s="0" t="inlineStr">
-        <is>
-          <t>Incorporate user documentation feedback</t>
-        </is>
-      </c>
-      <c r="B38" s="0" t="inlineStr">
-        <is>
-          <t>Technical Communicators</t>
-        </is>
-      </c>
-      <c r="C38" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D38" s="0" t="inlineStr">
-        <is>
-          <t>16h</t>
-        </is>
-      </c>
-      <c r="E38" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="39">
-      <c r="A39" s="0" t="inlineStr">
-        <is>
-          <t>Determine final deployment strategy</t>
-        </is>
-      </c>
-      <c r="B39" s="0" t="inlineStr">
-        <is>
-          <t>Deployment Team</t>
-        </is>
-      </c>
-      <c r="C39" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D39" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E39" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="40">
-      <c r="A40" s="0" t="inlineStr">
-        <is>
-          <t>Develop deployment methodology</t>
-        </is>
-      </c>
-      <c r="B40" s="0" t="inlineStr">
-        <is>
-          <t>Deployment Team</t>
-        </is>
-      </c>
-      <c r="C40" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D40" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E40" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="41">
-      <c r="A41" s="0" t="inlineStr">
-        <is>
-          <t>Secure deployment resources</t>
-        </is>
-      </c>
-      <c r="B41" s="0" t="inlineStr">
-        <is>
-          <t>Deployment Team</t>
-        </is>
-      </c>
-      <c r="C41" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D41" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E41" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="42">
-      <c r="A42" s="0" t="inlineStr">
-        <is>
-          <t>Train support staff</t>
-        </is>
-      </c>
-      <c r="B42" s="0" t="inlineStr">
-        <is>
-          <t>Deployment Team</t>
-        </is>
-      </c>
-      <c r="C42" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D42" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E42" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="43">
-      <c r="A43" s="0" t="inlineStr">
-        <is>
-          <t>Deploy software</t>
-        </is>
-      </c>
-      <c r="B43" s="0" t="inlineStr">
-        <is>
-          <t>Deployment Team</t>
-        </is>
-      </c>
-      <c r="C43" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D43" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E43" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="44">
-      <c r="A44" s="0" t="inlineStr">
-        <is>
-          <t>Document lessons learned</t>
-        </is>
-      </c>
-      <c r="B44" s="0" t="inlineStr">
-        <is>
-          <t>Project Manager</t>
-        </is>
-      </c>
-      <c r="C44" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D44" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E44" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="45">
-      <c r="A45" s="0" t="inlineStr">
-        <is>
-          <t>Distribute to team members</t>
-        </is>
-      </c>
-      <c r="B45" s="0" t="inlineStr">
-        <is>
-          <t>Project Manager</t>
-        </is>
-      </c>
-      <c r="C45" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D45" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E45" s="0" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="46">
-      <c r="A46" s="0" t="inlineStr">
-        <is>
-          <t>Create software maintenance team</t>
-        </is>
-      </c>
-      <c r="B46" s="0" t="inlineStr">
-        <is>
-          <t>Project Manager</t>
-        </is>
-      </c>
-      <c r="C46" s="0" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D46" s="0" t="inlineStr">
-        <is>
-          <t>8h</t>
-        </is>
-      </c>
-      <c r="E46" s="0" t="inlineStr">
         <is>
           <t>100%</t>
         </is>

</xml_diff>